<commit_message>
adjusted the car network as well
</commit_message>
<xml_diff>
--- a/Data_files/Rotterdam_train_adjacency.xlsx
+++ b/Data_files/Rotterdam_train_adjacency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD71ED-0FD7-45DD-BDA4-B27BFD071513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F9E81E-35FD-4112-8E9E-3E92018A024B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6430" yWindow="3710" windowWidth="19170" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Locations</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Schiedam</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Employees</t>
   </si>
 </sst>
 </file>
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +488,7 @@
     <col min="1" max="1" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,53 +498,59 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
       </c>
       <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
         <v>2</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <v>3</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <v>4</v>
       </c>
-      <c r="I1">
+      <c r="K1">
         <v>5</v>
       </c>
-      <c r="J1">
+      <c r="L1">
         <v>6</v>
       </c>
-      <c r="K1">
+      <c r="M1">
         <v>7</v>
       </c>
-      <c r="L1">
+      <c r="N1">
         <v>8</v>
       </c>
-      <c r="M1">
+      <c r="O1">
         <v>9</v>
       </c>
-      <c r="N1">
+      <c r="P1">
         <v>10</v>
       </c>
-      <c r="O1">
+      <c r="Q1">
         <v>11</v>
       </c>
-      <c r="P1">
+      <c r="R1">
         <v>12</v>
       </c>
-      <c r="Q1">
+      <c r="S1">
         <v>13</v>
       </c>
-      <c r="R1">
+      <c r="T1">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,17 +561,17 @@
         <v>4.3628</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" cm="1">
-        <f t="array" ref="E2:R2">TRANSPOSE(D3:D16)</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
+        <v>106086</v>
+      </c>
+      <c r="E2">
+        <v>111.3943676</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" cm="1">
+        <f t="array" ref="G2:T2">TRANSPOSE(F3:F16)</f>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
@@ -568,34 +580,40 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
+      <c r="S2" s="1">
+        <v>1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -606,19 +624,19 @@
         <v>4.3007</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>562839</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" cm="1">
-        <f t="array" ref="F3:R3">TRANSPOSE(E4:E16)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
+        <v>591.0025306</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" cm="1">
+        <f t="array" ref="H3:T3">TRANSPOSE(G4:G16)</f>
         <v>0</v>
       </c>
       <c r="I3" s="1">
@@ -646,13 +664,19 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -663,23 +687,23 @@
         <v>4.6905000000000001</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>121434</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>127.5103561</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" s="1" cm="1">
-        <f t="array" ref="G4:R4">TRANSPOSE(F5:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" cm="1">
+        <f t="array" ref="I4:T4">TRANSPOSE(H5:H16)</f>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -691,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -708,8 +732,14 @@
       <c r="R4" s="1">
         <v>0</v>
       </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -720,10 +750,10 @@
         <v>4.7083000000000004</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>75316</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>79.084687790000004</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -731,15 +761,15 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="1" cm="1">
-        <f t="array" ref="H5:R5">TRANSPOSE(G6:G16)</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" cm="1">
+        <f t="array" ref="J5:T5">TRANSPOSE(I6:I16)</f>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -763,10 +793,16 @@
         <v>0</v>
       </c>
       <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -777,28 +813,28 @@
         <v>4.5518999999999998</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>110650</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" s="1" cm="1">
-        <f t="array" ref="I6:R6">TRANSPOSE(H7:H16)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" cm="1">
+        <f t="array" ref="K6:T6">TRANSPOSE(J7:J16)</f>
         <v>0</v>
       </c>
       <c r="L6" s="1">
@@ -808,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
@@ -822,8 +858,14 @@
       <c r="R6" s="1">
         <v>0</v>
       </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -834,44 +876,44 @@
         <v>4.4890999999999996</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>110650</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" s="1" cm="1">
-        <f t="array" ref="J7:R7">TRANSPOSE(I8:I16)</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" cm="1">
+        <f t="array" ref="L7:T7">TRANSPOSE(K8:K16)</f>
+        <v>1</v>
       </c>
       <c r="M7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="1">
         <v>0</v>
@@ -879,8 +921,14 @@
       <c r="R7" s="1">
         <v>0</v>
       </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -891,34 +939,34 @@
         <v>4.4794</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>110650</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1" cm="1">
-        <f t="array" ref="K8:R8">TRANSPOSE(J9:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" cm="1">
+        <f t="array" ref="M8:T8">TRANSPOSE(L9:L16)</f>
         <v>0</v>
       </c>
       <c r="N8" s="1">
@@ -928,7 +976,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="1">
         <v>0</v>
@@ -936,8 +984,14 @@
       <c r="R8" s="1">
         <v>0</v>
       </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -948,19 +1002,19 @@
         <v>4.5313999999999997</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>110650</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -971,18 +1025,18 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9" s="1" cm="1">
-        <f t="array" ref="L9:R9">TRANSPOSE(K10:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" cm="1">
+        <f t="array" ref="N9:T9">TRANSPOSE(M10:M16)</f>
         <v>0</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
@@ -993,8 +1047,14 @@
       <c r="R9" s="1">
         <v>0</v>
       </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1005,10 +1065,10 @@
         <v>4.4814999999999996</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>110650</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1017,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1029,16 +1089,16 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" cm="1">
-        <f t="array" ref="M10:R10">TRANSPOSE(L11:L16)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" cm="1">
+        <f t="array" ref="O10:T10">TRANSPOSE(N11:N16)</f>
         <v>0</v>
       </c>
       <c r="P10" s="1">
@@ -1050,8 +1110,14 @@
       <c r="R10" s="1">
         <v>0</v>
       </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1062,10 +1128,10 @@
         <v>4.5098000000000003</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>110650</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>116.1867426</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1077,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1089,16 +1155,16 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" s="1" cm="1">
-        <f t="array" ref="N11:R11">TRANSPOSE(M12:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" cm="1">
+        <f t="array" ref="P11:T11">TRANSPOSE(O12:O16)</f>
         <v>0</v>
       </c>
       <c r="Q11" s="1">
@@ -1107,8 +1173,14 @@
       <c r="R11" s="1">
         <v>0</v>
       </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1119,13 +1191,13 @@
         <v>4.4098035896042003</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>77999</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>81.901940670000002</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1134,16 +1206,16 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1151,21 +1223,27 @@
       <c r="N12">
         <v>0</v>
       </c>
-      <c r="O12" s="1" cm="1">
-        <f t="array" ref="O12:R12">TRANSPOSE(N13:N16)</f>
-        <v>1</v>
-      </c>
-      <c r="P12" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" cm="1">
+        <f t="array" ref="Q12:T12">TRANSPOSE(P13:P16)</f>
         <v>1</v>
       </c>
       <c r="R12" s="1">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>1</v>
+      </c>
+      <c r="T12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1176,10 +1254,10 @@
         <v>4.3212999999999999</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>72561</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>76.191832160000004</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1206,23 +1284,29 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13" s="1" cm="1">
-        <f t="array" ref="P13:R13">TRANSPOSE(O14:O16)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>0</v>
-      </c>
-      <c r="R13" s="1">
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" cm="1">
+        <f t="array" ref="R13:T13">TRANSPOSE(Q14:Q16)</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1233,10 +1317,10 @@
         <v>4.3623000000000003</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>75079</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>78.835828710000001</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1263,23 +1347,29 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1" cm="1">
-        <f t="array" ref="Q14:R14">TRANSPOSE(P15:P16)</f>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14" s="1">
         <v>0</v>
       </c>
+      <c r="S14" s="1" cm="1">
+        <f t="array" ref="S14:T14">TRANSPOSE(R15:R16)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1290,16 +1380,16 @@
         <v>4.2088999999999999</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>114887</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>120.635755</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1320,23 +1410,29 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="R15" s="1" cm="1">
-        <f t="array" ref="R15">TRANSPOSE(Q16)</f>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1" cm="1">
+        <f t="array" ref="T15">TRANSPOSE(S16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1347,10 +1443,10 @@
         <v>4.4936999999999996</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>126998</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>133.3527694</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1362,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1389,6 +1485,12 @@
         <v>0</v>
       </c>
       <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
         <v>0</v>
       </c>
     </row>
@@ -1398,9 +1500,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1548,19 +1653,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6184B6F-9C77-4F99-9C89-9DA6F4E4B4A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A916EAA-9C41-45E2-9615-1537E158943C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1584,9 +1685,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A916EAA-9C41-45E2-9615-1537E158943C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6184B6F-9C77-4F99-9C89-9DA6F4E4B4A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>